<commit_message>
- updated data - new experimentations
</commit_message>
<xml_diff>
--- a/data/in/demo.xlsx
+++ b/data/in/demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\personal-finance-for-newbies\data\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14E3806-39C5-49EB-8767-F70D8FF81F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53723B8A-1087-4785-9506-8408B0EBA732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
   <si>
     <t>Exchange</t>
   </si>
@@ -351,8 +351,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella1" displayName="Tabella1" ref="A1:F36" totalsRowShown="0">
-  <autoFilter ref="A1:F36" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella1" displayName="Tabella1" ref="A1:F37" totalsRowShown="0">
+  <autoFilter ref="A1:F37" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Exchange"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ticker"/>
@@ -676,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1413,6 +1413,61 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="6">
+        <v>45231</v>
+      </c>
+      <c r="D37" s="5">
+        <v>46</v>
+      </c>
+      <c r="E37" s="2">
+        <v>13.638</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1427,7 +1482,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
update securities master table
</commit_message>
<xml_diff>
--- a/data/in/demo.xlsx
+++ b/data/in/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\personal-finance-for-newbies\data\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E70308-B59F-485F-89F5-F3DFB4F28498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE0865A-E4D2-4D36-B9BC-0CC61232EB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions History" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="52">
   <si>
     <t>Exchange</t>
   </si>
@@ -181,15 +181,6 @@
   </si>
   <si>
     <t>LCCN</t>
-  </si>
-  <si>
-    <t>BTCE</t>
-  </si>
-  <si>
-    <t>Bitcoin</t>
-  </si>
-  <si>
-    <t>ETC Group Physical Bitcoin</t>
   </si>
   <si>
     <t>Amundi Euro Government Inflation Linked Bond</t>
@@ -446,8 +437,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="AnagraficaTitoli" displayName="AnagraficaTitoli" ref="A1:E17" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="AnagraficaTitoli" displayName="AnagraficaTitoli" ref="A1:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Exchange" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Ticker" dataDxfId="3"/>
@@ -758,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -1884,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1924,7 +1915,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>24</v>
@@ -1941,7 +1932,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>26</v>
@@ -2111,7 +2102,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>43</v>
@@ -2162,30 +2153,13 @@
         <v>47</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>